<commit_message>
New script created and updated readme file. Took a look at timeline, accidentally changed the date but changed it back
</commit_message>
<xml_diff>
--- a/Expt - LPS biopsy GTT Spring 2021 study timeline revised.xlsx
+++ b/Expt - LPS biopsy GTT Spring 2021 study timeline revised.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\claud\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usu-my.sharepoint.com/personal/a02308724_aggies_usu_edu/Documents/Desktop/ASU green iguana 2021/greeniguanaAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31962B21-E157-446A-934F-03EB16C15E02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{31962B21-E157-446A-934F-03EB16C15E02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB48FF41-4743-4E6E-9BC7-D4BBE7E81AA9}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -925,7 +925,7 @@
   </sheetPr>
   <dimension ref="A1:AL12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F2" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="L2" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
new script and data
</commit_message>
<xml_diff>
--- a/Expt - LPS biopsy GTT Spring 2021 study timeline revised.xlsx
+++ b/Expt - LPS biopsy GTT Spring 2021 study timeline revised.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -925,8 +925,8 @@
   </sheetPr>
   <dimension ref="A1:AL12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L2" sqref="L1:L1048576"/>
+    <sheetView tabSelected="1" topLeftCell="S2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="X6" sqref="X6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>